<commit_message>
Add a ps1 file to remove old logs
</commit_message>
<xml_diff>
--- a/Office/九九加法表.xlsx
+++ b/Office/九九加法表.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PersonalRepo\Office\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="九九乘法表" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">九九乘法表!$A$1:$J$10</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -112,6 +115,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -159,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,7 +200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,7 +415,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -828,28 +834,4 @@
     <brk id="10" max="36" man="1"/>
   </colBreaks>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>